<commit_message>
Added raw 2020 Paris results
</commit_message>
<xml_diff>
--- a/data/raw_election_results_1st_round/munic2014-ardmnt.xlsx
+++ b/data/raw_election_results_1st_round/munic2014-ardmnt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexandreandorra/repos/pollsposition_models/fondamentaux/data/election_results_1st_round/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex_andorra/repos/pollsposition_models/data/raw_election_results_1st_round/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB2E66B-966F-1F48-8FD6-814AA590DD57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3375C298-CE5C-B145-96C3-5A6EA3E8C79B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="280" yWindow="540" windowWidth="25040" windowHeight="14080" xr2:uid="{DD182FFE-F7A7-2B4D-B46F-FD583BE3D052}"/>
+    <workbookView xWindow="280" yWindow="540" windowWidth="33320" windowHeight="19220" xr2:uid="{DD182FFE-F7A7-2B4D-B46F-FD583BE3D052}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -2701,13 +2701,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24EAEA38-A55A-B443-A850-5B153BC28AD9}">
   <dimension ref="A1:EH38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:138" x14ac:dyDescent="0.2">

</xml_diff>